<commit_message>
Modified to parse from XML file and get on rate over diacom.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drshottt\PycharmProjects\Api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F0E8E7F5-112F-452E-B13D-B200F9A985A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{037A883A-DA79-4927-B046-626C2D44CDF3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{AE46D11F-B078-4E80-8F01-95F4CAF886A0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>L Smith</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Rawdon</t>
   </si>
   <si>
-    <t>QC</t>
-  </si>
-  <si>
     <t>Daniel Burkholder</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Burns Lake</t>
   </si>
   <si>
-    <t>BC</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -66,12 +60,6 @@
     <t>zip</t>
   </si>
   <si>
-    <t>J0K1S0</t>
-  </si>
-  <si>
-    <t>V0J1E2</t>
-  </si>
-  <si>
     <t>serviceid</t>
   </si>
   <si>
@@ -85,6 +73,15 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>L4L4Y8</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>L7E4G4</t>
   </si>
 </sst>
 </file>
@@ -439,41 +436,48 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -487,27 +491,27 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>